<commit_message>
Updated by the robot
</commit_message>
<xml_diff>
--- a/covid_19_data_switzerland-phase2.xlsx
+++ b/covid_19_data_switzerland-phase2.xlsx
@@ -593,7 +593,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1210</v>
+        <v>9</v>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
@@ -667,11 +667,11 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1213</v>
+        <v>12</v>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
         <v>1</v>
@@ -689,7 +689,7 @@
         <v>4</v>
       </c>
       <c r="J4" t="n">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="K4" t="n">
         <v>1</v>
@@ -707,14 +707,14 @@
         <v>0</v>
       </c>
       <c r="P4" t="n">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="Q4" t="inlineStr"/>
       <c r="R4" t="n">
-        <v>78</v>
+        <v>0</v>
       </c>
       <c r="S4" t="n">
-        <v>443</v>
+        <v>3</v>
       </c>
       <c r="T4" t="n">
         <v>0</v>
@@ -751,13 +751,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1213</v>
+        <v>12</v>
       </c>
       <c r="C5" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
         <v>2</v>
@@ -775,7 +775,7 @@
         <v>6</v>
       </c>
       <c r="J5" t="n">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
         <v>1</v>
@@ -793,16 +793,16 @@
         <v>0</v>
       </c>
       <c r="P5" t="n">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="Q5" t="n">
-        <v>809</v>
+        <v>1</v>
       </c>
       <c r="R5" t="n">
-        <v>78</v>
+        <v>0</v>
       </c>
       <c r="S5" t="n">
-        <v>445</v>
+        <v>5</v>
       </c>
       <c r="T5" t="n">
         <v>0</v>
@@ -837,11 +837,11 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1216</v>
+        <v>15</v>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
         <v>4</v>
@@ -859,7 +859,7 @@
         <v>7</v>
       </c>
       <c r="J6" t="n">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="K6" t="n">
         <v>1</v>
@@ -877,14 +877,14 @@
         <v>0</v>
       </c>
       <c r="P6" t="n">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="Q6" t="inlineStr"/>
       <c r="R6" t="n">
-        <v>78</v>
+        <v>0</v>
       </c>
       <c r="S6" t="n">
-        <v>446</v>
+        <v>6</v>
       </c>
       <c r="T6" t="n">
         <v>0</v>
@@ -920,10 +920,10 @@
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
         <v>6</v>
@@ -941,7 +941,7 @@
         <v>8</v>
       </c>
       <c r="J7" t="n">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="K7" t="n">
         <v>1</v>
@@ -959,14 +959,14 @@
         <v>0</v>
       </c>
       <c r="P7" t="n">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="Q7" t="inlineStr"/>
       <c r="R7" t="n">
-        <v>78</v>
+        <v>0</v>
       </c>
       <c r="S7" t="n">
-        <v>446</v>
+        <v>6</v>
       </c>
       <c r="T7" t="n">
         <v>0</v>
@@ -1139,11 +1139,11 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1218</v>
+        <v>17</v>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
         <v>8</v>
@@ -1161,7 +1161,7 @@
         <v>12</v>
       </c>
       <c r="J10" t="n">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="K10" t="n">
         <v>1</v>
@@ -1179,14 +1179,14 @@
         <v>0</v>
       </c>
       <c r="P10" t="n">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="Q10" t="inlineStr"/>
       <c r="R10" t="n">
-        <v>79</v>
+        <v>1</v>
       </c>
       <c r="S10" t="n">
-        <v>446</v>
+        <v>6</v>
       </c>
       <c r="T10" t="n">
         <v>0</v>
@@ -1221,10 +1221,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1220</v>
+        <v>19</v>
       </c>
       <c r="C11" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="n">
@@ -1243,7 +1243,7 @@
         <v>12</v>
       </c>
       <c r="J11" t="n">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="K11" t="n">
         <v>1</v>
@@ -1261,14 +1261,14 @@
         <v>0</v>
       </c>
       <c r="P11" t="n">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="Q11" t="inlineStr"/>
       <c r="R11" t="n">
-        <v>79</v>
+        <v>1</v>
       </c>
       <c r="S11" t="n">
-        <v>446</v>
+        <v>6</v>
       </c>
       <c r="T11" t="n">
         <v>0</v>
@@ -1303,10 +1303,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1220</v>
+        <v>19</v>
       </c>
       <c r="C12" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="n">
@@ -1325,7 +1325,7 @@
         <v>12</v>
       </c>
       <c r="J12" t="n">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="K12" t="n">
         <v>2</v>
@@ -1343,13 +1343,13 @@
         <v>0</v>
       </c>
       <c r="P12" t="n">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="Q12" t="n">
-        <v>811</v>
+        <v>3</v>
       </c>
       <c r="R12" t="n">
-        <v>79</v>
+        <v>1</v>
       </c>
       <c r="S12" t="inlineStr"/>
       <c r="T12" t="n">
@@ -1385,7 +1385,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1222</v>
+        <v>21</v>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
@@ -1405,7 +1405,7 @@
         <v>12</v>
       </c>
       <c r="J13" t="n">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="K13" t="n">
         <v>3</v>
@@ -1425,7 +1425,7 @@
       <c r="P13" t="inlineStr"/>
       <c r="Q13" t="inlineStr"/>
       <c r="R13" t="n">
-        <v>79</v>
+        <v>1</v>
       </c>
       <c r="S13" t="inlineStr"/>
       <c r="T13" t="n">
@@ -1462,10 +1462,10 @@
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E14" t="n">
         <v>17</v>
@@ -1483,7 +1483,7 @@
         <v>16</v>
       </c>
       <c r="J14" t="n">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="K14" t="n">
         <v>3</v>
@@ -1501,7 +1501,7 @@
       <c r="P14" t="inlineStr"/>
       <c r="Q14" t="inlineStr"/>
       <c r="R14" t="n">
-        <v>79</v>
+        <v>1</v>
       </c>
       <c r="S14" t="inlineStr"/>
       <c r="T14" t="n">
@@ -1537,7 +1537,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1226</v>
+        <v>25</v>
       </c>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
@@ -1605,7 +1605,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1227</v>
+        <v>26</v>
       </c>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
@@ -1642,7 +1642,7 @@
       <c r="Q16" t="inlineStr"/>
       <c r="R16" t="inlineStr"/>
       <c r="S16" t="n">
-        <v>448</v>
+        <v>8</v>
       </c>
       <c r="T16" t="n">
         <v>1</v>
@@ -1677,11 +1677,11 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1229</v>
+        <v>28</v>
       </c>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="n">
@@ -1697,7 +1697,7 @@
         <v>18</v>
       </c>
       <c r="J17" t="n">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="K17" t="n">
         <v>3</v>
@@ -1713,14 +1713,14 @@
         <v>0</v>
       </c>
       <c r="P17" t="n">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="Q17" t="inlineStr"/>
       <c r="R17" t="n">
-        <v>81</v>
+        <v>3</v>
       </c>
       <c r="S17" t="n">
-        <v>448</v>
+        <v>8</v>
       </c>
       <c r="T17" t="n">
         <v>1</v>
@@ -1755,10 +1755,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1230</v>
+        <v>29</v>
       </c>
       <c r="C18" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr"/>
@@ -1775,7 +1775,7 @@
         <v>18</v>
       </c>
       <c r="J18" t="n">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="K18" t="n">
         <v>3</v>
@@ -1793,14 +1793,14 @@
         <v>0</v>
       </c>
       <c r="P18" t="n">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="Q18" t="inlineStr"/>
       <c r="R18" t="n">
-        <v>81</v>
+        <v>3</v>
       </c>
       <c r="S18" t="n">
-        <v>448</v>
+        <v>8</v>
       </c>
       <c r="T18" t="n">
         <v>1</v>
@@ -1835,10 +1835,10 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>1231</v>
+        <v>30</v>
       </c>
       <c r="C19" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr"/>
@@ -1853,7 +1853,7 @@
       </c>
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="n">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="K19" t="n">
         <v>3</v>
@@ -1871,16 +1871,16 @@
         <v>0</v>
       </c>
       <c r="P19" t="n">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="Q19" t="n">
-        <v>820</v>
+        <v>12</v>
       </c>
       <c r="R19" t="n">
-        <v>81</v>
+        <v>3</v>
       </c>
       <c r="S19" t="n">
-        <v>449</v>
+        <v>9</v>
       </c>
       <c r="T19" t="n">
         <v>1</v>
@@ -1915,7 +1915,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1231</v>
+        <v>30</v>
       </c>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr"/>
@@ -1931,7 +1931,7 @@
       </c>
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="n">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="K20" t="n">
         <v>3</v>
@@ -1949,14 +1949,14 @@
         <v>0</v>
       </c>
       <c r="P20" t="n">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="Q20" t="inlineStr"/>
       <c r="R20" t="n">
-        <v>81</v>
+        <v>3</v>
       </c>
       <c r="S20" t="n">
-        <v>449</v>
+        <v>9</v>
       </c>
       <c r="T20" t="n">
         <v>1</v>
@@ -1991,13 +1991,13 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1235</v>
+        <v>34</v>
       </c>
       <c r="C21" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="n">
@@ -2011,7 +2011,7 @@
       </c>
       <c r="I21" t="inlineStr"/>
       <c r="J21" t="n">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="K21" t="n">
         <v>3</v>
@@ -2029,14 +2029,14 @@
         <v>0</v>
       </c>
       <c r="P21" t="n">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="Q21" t="inlineStr"/>
       <c r="R21" t="n">
-        <v>81</v>
+        <v>3</v>
       </c>
       <c r="S21" t="n">
-        <v>451</v>
+        <v>11</v>
       </c>
       <c r="T21" t="n">
         <v>2</v>
@@ -2203,11 +2203,11 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>1239</v>
+        <v>38</v>
       </c>
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="n">
@@ -2221,7 +2221,7 @@
       </c>
       <c r="I24" t="inlineStr"/>
       <c r="J24" t="n">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="K24" t="n">
         <v>4</v>
@@ -2239,16 +2239,16 @@
         <v>0</v>
       </c>
       <c r="P24" t="n">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="Q24" t="n">
-        <v>822</v>
+        <v>14</v>
       </c>
       <c r="R24" t="n">
-        <v>81</v>
+        <v>3</v>
       </c>
       <c r="S24" t="n">
-        <v>451</v>
+        <v>11</v>
       </c>
       <c r="T24" t="n">
         <v>6</v>
@@ -2283,10 +2283,10 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>1241</v>
+        <v>40</v>
       </c>
       <c r="C25" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr"/>
@@ -2301,7 +2301,7 @@
       </c>
       <c r="I25" t="inlineStr"/>
       <c r="J25" t="n">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="K25" t="n">
         <v>4</v>
@@ -2319,16 +2319,16 @@
         <v>0</v>
       </c>
       <c r="P25" t="n">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="Q25" t="n">
-        <v>823</v>
+        <v>15</v>
       </c>
       <c r="R25" t="n">
-        <v>81</v>
+        <v>3</v>
       </c>
       <c r="S25" t="n">
-        <v>451</v>
+        <v>11</v>
       </c>
       <c r="T25" t="n">
         <v>6</v>
@@ -2363,10 +2363,10 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>1241</v>
+        <v>40</v>
       </c>
       <c r="C26" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr"/>
@@ -2381,7 +2381,7 @@
       </c>
       <c r="I26" t="inlineStr"/>
       <c r="J26" t="n">
-        <v>129</v>
+        <v>1</v>
       </c>
       <c r="K26" t="n">
         <v>4</v>
@@ -2397,14 +2397,14 @@
         <v>0</v>
       </c>
       <c r="P26" t="n">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="Q26" t="n">
-        <v>825</v>
+        <v>17</v>
       </c>
       <c r="R26" t="inlineStr"/>
       <c r="S26" t="n">
-        <v>452</v>
+        <v>12</v>
       </c>
       <c r="T26" t="n">
         <v>9</v>
@@ -2439,11 +2439,11 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>1248</v>
+        <v>47</v>
       </c>
       <c r="C27" t="inlineStr"/>
       <c r="D27" t="n">
-        <v>101</v>
+        <v>1</v>
       </c>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="n">
@@ -2457,7 +2457,7 @@
       </c>
       <c r="I27" t="inlineStr"/>
       <c r="J27" t="n">
-        <v>129</v>
+        <v>1</v>
       </c>
       <c r="K27" t="n">
         <v>4</v>
@@ -2473,14 +2473,14 @@
         <v>0</v>
       </c>
       <c r="P27" t="n">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="Q27" t="n">
-        <v>828</v>
+        <v>20</v>
       </c>
       <c r="R27" t="inlineStr"/>
       <c r="S27" t="n">
-        <v>453</v>
+        <v>13</v>
       </c>
       <c r="T27" t="n">
         <v>10</v>
@@ -2513,13 +2513,13 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>1254</v>
+        <v>53</v>
       </c>
       <c r="C28" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>101</v>
+        <v>1</v>
       </c>
       <c r="E28" t="n">
         <v>18</v>
@@ -2535,7 +2535,7 @@
       </c>
       <c r="I28" t="inlineStr"/>
       <c r="J28" t="n">
-        <v>129</v>
+        <v>1</v>
       </c>
       <c r="K28" t="inlineStr"/>
       <c r="L28" t="inlineStr"/>
@@ -2545,14 +2545,14 @@
       <c r="N28" t="inlineStr"/>
       <c r="O28" t="inlineStr"/>
       <c r="P28" t="n">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="Q28" t="n">
-        <v>831</v>
+        <v>23</v>
       </c>
       <c r="R28" t="inlineStr"/>
       <c r="S28" t="n">
-        <v>453</v>
+        <v>13</v>
       </c>
       <c r="T28" t="n">
         <v>13</v>
@@ -2972,11 +2972,11 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -2994,7 +2994,7 @@
         <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="K4" t="n">
         <v>0</v>
@@ -3016,10 +3016,10 @@
       </c>
       <c r="Q4" t="inlineStr"/>
       <c r="R4" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S4" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="T4" t="n">
         <v>0</v>
@@ -3060,7 +3060,7 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
@@ -3078,7 +3078,7 @@
         <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
         <v>0</v>
@@ -3099,13 +3099,13 @@
         <v>0</v>
       </c>
       <c r="Q5" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="R5" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S5" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="T5" t="n">
         <v>0</v>
@@ -3140,11 +3140,11 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -3162,7 +3162,7 @@
         <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="K6" t="n">
         <v>0</v>
@@ -3184,10 +3184,10 @@
       </c>
       <c r="Q6" t="inlineStr"/>
       <c r="R6" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S6" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="T6" t="n">
         <v>0</v>
@@ -3226,7 +3226,7 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -3244,7 +3244,7 @@
         <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="K7" t="n">
         <v>0</v>
@@ -3266,10 +3266,10 @@
       </c>
       <c r="Q7" t="inlineStr"/>
       <c r="R7" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S7" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="T7" t="n">
         <v>0</v>
@@ -3442,11 +3442,11 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -3464,7 +3464,7 @@
         <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="K10" t="n">
         <v>1</v>
@@ -3486,10 +3486,10 @@
       </c>
       <c r="Q10" t="inlineStr"/>
       <c r="R10" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="S10" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="T10" t="n">
         <v>0</v>
@@ -3544,7 +3544,7 @@
         <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="K11" t="n">
         <v>1</v>
@@ -3566,10 +3566,10 @@
       </c>
       <c r="Q11" t="inlineStr"/>
       <c r="R11" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="S11" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="T11" t="n">
         <v>0</v>
@@ -3624,7 +3624,7 @@
         <v>1</v>
       </c>
       <c r="J12" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="K12" t="n">
         <v>1</v>
@@ -3645,10 +3645,10 @@
         <v>0</v>
       </c>
       <c r="Q12" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="R12" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="S12" t="inlineStr"/>
       <c r="T12" t="n">
@@ -3684,7 +3684,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
@@ -3704,7 +3704,7 @@
         <v>1</v>
       </c>
       <c r="J13" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="K13" t="n">
         <v>1</v>
@@ -3722,7 +3722,7 @@
       <c r="P13" t="inlineStr"/>
       <c r="Q13" t="inlineStr"/>
       <c r="R13" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="S13" t="inlineStr"/>
       <c r="T13" t="n">
@@ -3762,7 +3762,7 @@
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -3780,7 +3780,7 @@
         <v>1</v>
       </c>
       <c r="J14" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="K14" t="n">
         <v>1</v>
@@ -3796,7 +3796,7 @@
       <c r="P14" t="inlineStr"/>
       <c r="Q14" t="inlineStr"/>
       <c r="R14" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="S14" t="inlineStr"/>
       <c r="T14" t="n">
@@ -3933,7 +3933,7 @@
       <c r="Q16" t="inlineStr"/>
       <c r="R16" t="inlineStr"/>
       <c r="S16" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="T16" t="n">
         <v>0</v>
@@ -3970,7 +3970,7 @@
       <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E17" t="n">
         <v>0</v>
@@ -3988,7 +3988,7 @@
         <v>1</v>
       </c>
       <c r="J17" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="K17" t="n">
         <v>1</v>
@@ -4006,10 +4006,10 @@
       </c>
       <c r="Q17" t="inlineStr"/>
       <c r="R17" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="S17" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="T17" t="n">
         <v>0</v>
@@ -4062,7 +4062,7 @@
       </c>
       <c r="I18" t="inlineStr"/>
       <c r="J18" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="K18" t="n">
         <v>1</v>
@@ -4082,10 +4082,10 @@
       </c>
       <c r="Q18" t="inlineStr"/>
       <c r="R18" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="S18" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="T18" t="n">
         <v>0</v>
@@ -4138,7 +4138,7 @@
       </c>
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="K19" t="n">
         <v>1</v>
@@ -4157,13 +4157,13 @@
         <v>0</v>
       </c>
       <c r="Q19" t="n">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="R19" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="S19" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="T19" t="n">
         <v>0</v>
@@ -4198,7 +4198,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr"/>
@@ -4216,7 +4216,7 @@
       </c>
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="K20" t="n">
         <v>1</v>
@@ -4236,10 +4236,10 @@
       </c>
       <c r="Q20" t="inlineStr"/>
       <c r="R20" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="S20" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="T20" t="n">
         <v>0</v>
@@ -4274,13 +4274,13 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E21" t="n">
         <v>0</v>
@@ -4296,7 +4296,7 @@
       </c>
       <c r="I21" t="inlineStr"/>
       <c r="J21" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="K21" t="n">
         <v>1</v>
@@ -4316,10 +4316,10 @@
       </c>
       <c r="Q21" t="inlineStr"/>
       <c r="R21" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="S21" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="T21" t="n">
         <v>0</v>
@@ -4486,11 +4486,11 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E24" t="n">
         <v>0</v>
@@ -4504,7 +4504,7 @@
       <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr"/>
       <c r="J24" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="K24" t="n">
         <v>1</v>
@@ -4523,13 +4523,13 @@
         <v>0</v>
       </c>
       <c r="Q24" t="n">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="R24" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="S24" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="T24" t="n">
         <v>0</v>
@@ -4564,7 +4564,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
@@ -4584,7 +4584,7 @@
       </c>
       <c r="I25" t="inlineStr"/>
       <c r="J25" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="K25" t="n">
         <v>1</v>
@@ -4603,13 +4603,13 @@
         <v>0</v>
       </c>
       <c r="Q25" t="n">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="R25" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="S25" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="T25" t="n">
         <v>0</v>
@@ -4644,7 +4644,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
@@ -4664,7 +4664,7 @@
       </c>
       <c r="I26" t="inlineStr"/>
       <c r="J26" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="K26" t="n">
         <v>1</v>
@@ -4683,11 +4683,11 @@
         <v>0</v>
       </c>
       <c r="Q26" t="n">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="R26" t="inlineStr"/>
       <c r="S26" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="T26" t="n">
         <v>0</v>
@@ -4722,11 +4722,11 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="C27" t="inlineStr"/>
       <c r="D27" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E27" t="n">
         <v>0</v>
@@ -4742,7 +4742,7 @@
       </c>
       <c r="I27" t="inlineStr"/>
       <c r="J27" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="K27" t="n">
         <v>1</v>
@@ -4761,11 +4761,11 @@
         <v>0</v>
       </c>
       <c r="Q27" t="n">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="R27" t="inlineStr"/>
       <c r="S27" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="T27" t="n">
         <v>0</v>
@@ -4798,13 +4798,13 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E28" t="n">
         <v>0</v>
@@ -4820,7 +4820,7 @@
       </c>
       <c r="I28" t="inlineStr"/>
       <c r="J28" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="K28" t="inlineStr"/>
       <c r="L28" t="inlineStr"/>
@@ -4833,11 +4833,11 @@
         <v>0</v>
       </c>
       <c r="Q28" t="n">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="R28" t="inlineStr"/>
       <c r="S28" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="T28" t="n">
         <v>0</v>
@@ -5245,11 +5245,11 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4</v>
+        <v>-2</v>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
         <v>-3</v>
@@ -5264,7 +5264,7 @@
         <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>131</v>
+        <v>0</v>
       </c>
       <c r="J4" t="n">
         <v>0</v>
@@ -5287,7 +5287,7 @@
       </c>
       <c r="Q4" t="inlineStr"/>
       <c r="R4" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="S4" t="inlineStr"/>
       <c r="T4" t="inlineStr"/>
@@ -5325,7 +5325,7 @@
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
         <v>-3</v>
@@ -5340,7 +5340,7 @@
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>125</v>
+        <v>-6</v>
       </c>
       <c r="J5" t="n">
         <v>0</v>
@@ -5352,7 +5352,7 @@
         <v>-2</v>
       </c>
       <c r="M5" t="n">
-        <v>20</v>
+        <v>-6</v>
       </c>
       <c r="N5" t="n">
         <v>0</v>
@@ -5364,10 +5364,10 @@
         <v>0</v>
       </c>
       <c r="Q5" t="n">
-        <v>8</v>
+        <v>-3</v>
       </c>
       <c r="R5" t="n">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="S5" t="inlineStr"/>
       <c r="T5" t="inlineStr"/>
@@ -5401,11 +5401,11 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
         <v>-3</v>
@@ -5420,7 +5420,7 @@
         <v>-1</v>
       </c>
       <c r="I6" t="n">
-        <v>122</v>
+        <v>-9</v>
       </c>
       <c r="J6" t="n">
         <v>0</v>
@@ -5443,7 +5443,7 @@
       </c>
       <c r="Q6" t="inlineStr"/>
       <c r="R6" t="n">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="S6" t="inlineStr"/>
       <c r="T6" t="inlineStr"/>
@@ -5479,7 +5479,7 @@
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
         <v>-4</v>
@@ -5494,7 +5494,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>118</v>
+        <v>-13</v>
       </c>
       <c r="J7" t="n">
         <v>0</v>
@@ -5517,7 +5517,7 @@
       </c>
       <c r="Q7" t="inlineStr"/>
       <c r="R7" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="S7" t="inlineStr"/>
       <c r="T7" t="inlineStr"/>
@@ -5679,11 +5679,11 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>4</v>
+        <v>-2</v>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E10" t="n">
         <v>-6</v>
@@ -5698,7 +5698,7 @@
         <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>115</v>
+        <v>-16</v>
       </c>
       <c r="J10" t="n">
         <v>0</v>
@@ -5710,7 +5710,7 @@
         <v>-2</v>
       </c>
       <c r="M10" t="n">
-        <v>5</v>
+        <v>-21</v>
       </c>
       <c r="N10" t="n">
         <v>0</v>
@@ -5722,10 +5722,10 @@
         <v>0</v>
       </c>
       <c r="Q10" t="n">
-        <v>9</v>
+        <v>-2</v>
       </c>
       <c r="R10" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="S10" t="inlineStr"/>
       <c r="T10" t="inlineStr"/>
@@ -5774,7 +5774,7 @@
         <v>-1</v>
       </c>
       <c r="I11" t="n">
-        <v>118</v>
+        <v>-13</v>
       </c>
       <c r="J11" t="n">
         <v>0</v>
@@ -5797,7 +5797,7 @@
       </c>
       <c r="Q11" t="inlineStr"/>
       <c r="R11" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="S11" t="inlineStr"/>
       <c r="T11" t="inlineStr"/>
@@ -5846,7 +5846,7 @@
         <v>-1</v>
       </c>
       <c r="I12" t="n">
-        <v>116</v>
+        <v>-15</v>
       </c>
       <c r="J12" t="n">
         <v>0</v>
@@ -5858,7 +5858,7 @@
         <v>-2</v>
       </c>
       <c r="M12" t="n">
-        <v>8</v>
+        <v>-18</v>
       </c>
       <c r="N12" t="n">
         <v>0</v>
@@ -5871,7 +5871,7 @@
       </c>
       <c r="Q12" t="inlineStr"/>
       <c r="R12" t="n">
-        <v>3</v>
+        <v>-2</v>
       </c>
       <c r="S12" t="inlineStr"/>
       <c r="T12" t="inlineStr"/>
@@ -5905,7 +5905,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>2</v>
+        <v>-4</v>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
@@ -5922,7 +5922,7 @@
         <v>-2</v>
       </c>
       <c r="I13" t="n">
-        <v>112</v>
+        <v>-19</v>
       </c>
       <c r="J13" t="n">
         <v>0</v>
@@ -5943,7 +5943,7 @@
       <c r="P13" t="inlineStr"/>
       <c r="Q13" t="inlineStr"/>
       <c r="R13" t="n">
-        <v>1</v>
+        <v>-4</v>
       </c>
       <c r="S13" t="inlineStr"/>
       <c r="T13" t="inlineStr"/>
@@ -5979,7 +5979,7 @@
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E14" t="n">
         <v>-8</v>
@@ -5994,7 +5994,7 @@
         <v>-1</v>
       </c>
       <c r="I14" t="n">
-        <v>113</v>
+        <v>-18</v>
       </c>
       <c r="J14" t="n">
         <v>0</v>
@@ -6015,7 +6015,7 @@
       <c r="P14" t="inlineStr"/>
       <c r="Q14" t="inlineStr"/>
       <c r="R14" t="n">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="S14" t="inlineStr"/>
       <c r="T14" t="inlineStr"/>
@@ -6136,7 +6136,7 @@
         <v>-2</v>
       </c>
       <c r="M16" t="n">
-        <v>8</v>
+        <v>-18</v>
       </c>
       <c r="N16" t="n">
         <v>1</v>
@@ -6181,7 +6181,7 @@
       <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17" t="n">
         <v>-8</v>
@@ -6196,7 +6196,7 @@
         <v>-2</v>
       </c>
       <c r="I17" t="n">
-        <v>106</v>
+        <v>-25</v>
       </c>
       <c r="J17" t="n">
         <v>0</v>
@@ -6218,10 +6218,10 @@
         <v>0</v>
       </c>
       <c r="Q17" t="n">
-        <v>7</v>
+        <v>-4</v>
       </c>
       <c r="R17" t="n">
-        <v>1</v>
+        <v>-4</v>
       </c>
       <c r="S17" t="inlineStr"/>
       <c r="T17" t="inlineStr"/>
@@ -6270,7 +6270,7 @@
         <v>-1</v>
       </c>
       <c r="I18" t="n">
-        <v>103</v>
+        <v>-28</v>
       </c>
       <c r="J18" t="n">
         <v>0</v>
@@ -6293,7 +6293,7 @@
       </c>
       <c r="Q18" t="inlineStr"/>
       <c r="R18" t="n">
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="S18" t="inlineStr"/>
       <c r="T18" t="inlineStr"/>
@@ -6352,7 +6352,7 @@
         <v>-2</v>
       </c>
       <c r="M19" t="n">
-        <v>13</v>
+        <v>-13</v>
       </c>
       <c r="N19" t="n">
         <v>0</v>
@@ -6365,7 +6365,7 @@
       </c>
       <c r="Q19" t="inlineStr"/>
       <c r="R19" t="n">
-        <v>1</v>
+        <v>-4</v>
       </c>
       <c r="S19" t="inlineStr"/>
       <c r="T19" t="inlineStr"/>
@@ -6424,7 +6424,7 @@
         <v>-2</v>
       </c>
       <c r="M20" t="n">
-        <v>13</v>
+        <v>-13</v>
       </c>
       <c r="N20" t="n">
         <v>0</v>
@@ -6437,7 +6437,7 @@
       </c>
       <c r="Q20" t="inlineStr"/>
       <c r="R20" t="n">
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="S20" t="inlineStr"/>
       <c r="T20" t="inlineStr"/>
@@ -6473,7 +6473,7 @@
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E21" t="n">
         <v>-6</v>
@@ -6498,7 +6498,7 @@
         <v>-3</v>
       </c>
       <c r="M21" t="n">
-        <v>9</v>
+        <v>-17</v>
       </c>
       <c r="N21" t="n">
         <v>3</v>
@@ -6511,7 +6511,7 @@
       </c>
       <c r="Q21" t="inlineStr"/>
       <c r="R21" t="n">
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="S21" t="inlineStr"/>
       <c r="T21" t="inlineStr"/>
@@ -6673,7 +6673,7 @@
       <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E24" t="n">
         <v>-7</v>
@@ -6698,7 +6698,7 @@
         <v>-3</v>
       </c>
       <c r="M24" t="n">
-        <v>9</v>
+        <v>-17</v>
       </c>
       <c r="N24" t="n">
         <v>0</v>
@@ -6711,7 +6711,7 @@
       </c>
       <c r="Q24" t="inlineStr"/>
       <c r="R24" t="n">
-        <v>3</v>
+        <v>-2</v>
       </c>
       <c r="S24" t="inlineStr"/>
       <c r="T24" t="inlineStr"/>
@@ -6781,7 +6781,7 @@
       </c>
       <c r="Q25" t="inlineStr"/>
       <c r="R25" t="n">
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="S25" t="inlineStr"/>
       <c r="T25" t="inlineStr"/>
@@ -6840,7 +6840,7 @@
         <v>-3</v>
       </c>
       <c r="M26" t="n">
-        <v>10</v>
+        <v>-16</v>
       </c>
       <c r="N26" t="n">
         <v>-1</v>
@@ -6852,7 +6852,7 @@
         <v>0</v>
       </c>
       <c r="Q26" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="R26" t="inlineStr"/>
       <c r="S26" t="inlineStr"/>
@@ -6889,7 +6889,7 @@
       <c r="B27" t="inlineStr"/>
       <c r="C27" t="inlineStr"/>
       <c r="D27" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E27" t="n">
         <v>-8</v>
@@ -6914,7 +6914,7 @@
         <v>-3</v>
       </c>
       <c r="M27" t="n">
-        <v>10</v>
+        <v>-16</v>
       </c>
       <c r="N27" t="n">
         <v>-1</v>
@@ -6959,7 +6959,7 @@
       <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E28" t="n">
         <v>-8</v>
@@ -7378,7 +7378,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="n">
@@ -7416,7 +7416,7 @@
       <c r="P4" t="inlineStr"/>
       <c r="Q4" t="inlineStr"/>
       <c r="R4" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="S4" t="inlineStr"/>
       <c r="T4" t="inlineStr"/>
@@ -7475,7 +7475,7 @@
         <v>-1</v>
       </c>
       <c r="M5" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N5" t="n">
         <v>0</v>
@@ -7485,10 +7485,10 @@
       </c>
       <c r="P5" t="inlineStr"/>
       <c r="Q5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R5" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="S5" t="inlineStr"/>
       <c r="T5" t="inlineStr"/>
@@ -7520,7 +7520,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="n">
@@ -7558,7 +7558,7 @@
       <c r="P6" t="inlineStr"/>
       <c r="Q6" t="inlineStr"/>
       <c r="R6" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="S6" t="inlineStr"/>
       <c r="T6" t="inlineStr"/>
@@ -7626,7 +7626,7 @@
       <c r="P7" t="inlineStr"/>
       <c r="Q7" t="inlineStr"/>
       <c r="R7" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="S7" t="inlineStr"/>
       <c r="T7" t="inlineStr"/>
@@ -7782,7 +7782,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="n">
@@ -7811,7 +7811,7 @@
         <v>-1</v>
       </c>
       <c r="M10" t="n">
-        <v>3</v>
+        <v>-2</v>
       </c>
       <c r="N10" t="n">
         <v>0</v>
@@ -7821,10 +7821,10 @@
       </c>
       <c r="P10" t="inlineStr"/>
       <c r="Q10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R10" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="S10" t="inlineStr"/>
       <c r="T10" t="inlineStr"/>
@@ -7890,7 +7890,7 @@
       <c r="P11" t="inlineStr"/>
       <c r="Q11" t="inlineStr"/>
       <c r="R11" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="S11" t="inlineStr"/>
       <c r="T11" t="inlineStr"/>
@@ -7947,7 +7947,7 @@
         <v>-1</v>
       </c>
       <c r="M12" t="n">
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="N12" t="n">
         <v>0</v>
@@ -7958,7 +7958,7 @@
       <c r="P12" t="inlineStr"/>
       <c r="Q12" t="inlineStr"/>
       <c r="R12" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="S12" t="inlineStr"/>
       <c r="T12" t="inlineStr"/>
@@ -7990,7 +7990,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
@@ -8026,7 +8026,7 @@
       <c r="P13" t="inlineStr"/>
       <c r="Q13" t="inlineStr"/>
       <c r="R13" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="S13" t="inlineStr"/>
       <c r="T13" t="inlineStr"/>
@@ -8094,7 +8094,7 @@
       <c r="P14" t="inlineStr"/>
       <c r="Q14" t="inlineStr"/>
       <c r="R14" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="S14" t="inlineStr"/>
       <c r="T14" t="inlineStr"/>
@@ -8211,7 +8211,7 @@
         <v>-1</v>
       </c>
       <c r="M16" t="n">
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="N16" t="n">
         <v>0</v>
@@ -8287,10 +8287,10 @@
       </c>
       <c r="P17" t="inlineStr"/>
       <c r="Q17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R17" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="S17" t="inlineStr"/>
       <c r="T17" t="inlineStr"/>
@@ -8356,7 +8356,7 @@
       <c r="P18" t="inlineStr"/>
       <c r="Q18" t="inlineStr"/>
       <c r="R18" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="S18" t="inlineStr"/>
       <c r="T18" t="inlineStr"/>
@@ -8411,7 +8411,7 @@
         <v>-1</v>
       </c>
       <c r="M19" t="n">
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="N19" t="n">
         <v>0</v>
@@ -8422,7 +8422,7 @@
       <c r="P19" t="inlineStr"/>
       <c r="Q19" t="inlineStr"/>
       <c r="R19" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="S19" t="inlineStr"/>
       <c r="T19" t="inlineStr"/>
@@ -8477,7 +8477,7 @@
         <v>-1</v>
       </c>
       <c r="M20" t="n">
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="N20" t="n">
         <v>0</v>
@@ -8488,7 +8488,7 @@
       <c r="P20" t="inlineStr"/>
       <c r="Q20" t="inlineStr"/>
       <c r="R20" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="S20" t="inlineStr"/>
       <c r="T20" t="inlineStr"/>
@@ -8545,7 +8545,7 @@
         <v>-1</v>
       </c>
       <c r="M21" t="n">
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="N21" t="n">
         <v>1</v>
@@ -8556,7 +8556,7 @@
       <c r="P21" t="inlineStr"/>
       <c r="Q21" t="inlineStr"/>
       <c r="R21" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="S21" t="inlineStr"/>
       <c r="T21" t="inlineStr"/>
@@ -8735,7 +8735,7 @@
         <v>-1</v>
       </c>
       <c r="M24" t="n">
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="N24" t="n">
         <v>0</v>
@@ -8746,7 +8746,7 @@
       <c r="P24" t="inlineStr"/>
       <c r="Q24" t="inlineStr"/>
       <c r="R24" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="S24" t="inlineStr"/>
       <c r="T24" t="inlineStr"/>
@@ -8810,7 +8810,7 @@
       <c r="P25" t="inlineStr"/>
       <c r="Q25" t="inlineStr"/>
       <c r="R25" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="S25" t="inlineStr"/>
       <c r="T25" t="inlineStr"/>
@@ -8865,7 +8865,7 @@
         <v>-1</v>
       </c>
       <c r="M26" t="n">
-        <v>1</v>
+        <v>-4</v>
       </c>
       <c r="N26" t="n">
         <v>0</v>
@@ -8875,7 +8875,7 @@
       </c>
       <c r="P26" t="inlineStr"/>
       <c r="Q26" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R26" t="inlineStr"/>
       <c r="S26" t="inlineStr"/>
@@ -8933,7 +8933,7 @@
         <v>-1</v>
       </c>
       <c r="M27" t="n">
-        <v>1</v>
+        <v>-4</v>
       </c>
       <c r="N27" t="n">
         <v>0</v>
@@ -9361,7 +9361,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
@@ -9467,7 +9467,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
@@ -9673,7 +9673,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
@@ -9831,7 +9831,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
@@ -10980,7 +10980,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1140</v>
+        <v>20</v>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
@@ -10995,7 +10995,7 @@
         <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>807</v>
+        <v>10</v>
       </c>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
@@ -11051,7 +11051,7 @@
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>811</v>
+        <v>14</v>
       </c>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
@@ -11061,7 +11061,7 @@
       <c r="O5" t="inlineStr"/>
       <c r="P5" t="inlineStr"/>
       <c r="Q5" t="n">
-        <v>223</v>
+        <v>6</v>
       </c>
       <c r="R5" t="inlineStr"/>
       <c r="S5" t="inlineStr"/>
@@ -11094,7 +11094,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1145</v>
+        <v>25</v>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
@@ -11109,7 +11109,7 @@
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>817</v>
+        <v>20</v>
       </c>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
@@ -11163,7 +11163,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>821</v>
+        <v>24</v>
       </c>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
@@ -11308,7 +11308,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1150</v>
+        <v>30</v>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
@@ -11331,7 +11331,7 @@
       <c r="O10" t="inlineStr"/>
       <c r="P10" t="inlineStr"/>
       <c r="Q10" t="n">
-        <v>223</v>
+        <v>6</v>
       </c>
       <c r="R10" t="inlineStr"/>
       <c r="S10" t="inlineStr"/>
@@ -11377,7 +11377,7 @@
         <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>826</v>
+        <v>29</v>
       </c>
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
@@ -11431,7 +11431,7 @@
         <v>0</v>
       </c>
       <c r="I12" t="n">
-        <v>831</v>
+        <v>34</v>
       </c>
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
@@ -11472,7 +11472,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1155</v>
+        <v>35</v>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
@@ -11487,7 +11487,7 @@
         <v>0</v>
       </c>
       <c r="I13" t="n">
-        <v>835</v>
+        <v>38</v>
       </c>
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr"/>
@@ -11541,7 +11541,7 @@
         <v>0</v>
       </c>
       <c r="I14" t="n">
-        <v>836</v>
+        <v>39</v>
       </c>
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
@@ -11699,7 +11699,7 @@
         <v>0</v>
       </c>
       <c r="I17" t="n">
-        <v>844</v>
+        <v>47</v>
       </c>
       <c r="J17" t="inlineStr"/>
       <c r="K17" t="inlineStr"/>
@@ -11709,7 +11709,7 @@
       <c r="O17" t="inlineStr"/>
       <c r="P17" t="inlineStr"/>
       <c r="Q17" t="n">
-        <v>223</v>
+        <v>6</v>
       </c>
       <c r="R17" t="inlineStr"/>
       <c r="S17" t="inlineStr"/>
@@ -11755,7 +11755,7 @@
         <v>0</v>
       </c>
       <c r="I18" t="n">
-        <v>847</v>
+        <v>50</v>
       </c>
       <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr"/>
@@ -11848,7 +11848,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1170</v>
+        <v>50</v>
       </c>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr"/>
@@ -12183,7 +12183,7 @@
       <c r="O26" t="inlineStr"/>
       <c r="P26" t="inlineStr"/>
       <c r="Q26" t="n">
-        <v>226</v>
+        <v>9</v>
       </c>
       <c r="R26" t="inlineStr"/>
       <c r="S26" t="inlineStr"/>

</xml_diff>